<commit_message>
updated the search query in the member search
- update the import functions
- made sure the organisation is being properly handled
</commit_message>
<xml_diff>
--- a/src/test/resources/member List sample.xlsx
+++ b/src/test/resources/member List sample.xlsx
@@ -430,10 +430,14 @@
   <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:44" s="1" customFormat="1">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
cleaned up the keystroke lookup
added a few more fields to display
</commit_message>
<xml_diff>
--- a/src/test/resources/member List sample.xlsx
+++ b/src/test/resources/member List sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>NSW</t>
   </si>
@@ -53,6 +53,21 @@
   </si>
   <si>
     <t>+61288145232</t>
+  </si>
+  <si>
+    <t>DD124</t>
+  </si>
+  <si>
+    <t>Joe Brennan2</t>
+  </si>
+  <si>
+    <t>Jane Brennan2</t>
+  </si>
+  <si>
+    <t>Brennan2</t>
+  </si>
+  <si>
+    <t>Brannan2</t>
   </si>
 </sst>
 </file>
@@ -427,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR2"/>
+  <dimension ref="A1:AR4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -580,10 +595,153 @@
       <c r="AQ2" s="3"/>
       <c r="AR2" s="2"/>
     </row>
+    <row r="3" spans="1:44" s="1" customFormat="1">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1235</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2769</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>88145232</v>
+      </c>
+      <c r="K3" s="1">
+        <v>407634768</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1966</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="3"/>
+      <c r="AP3" s="3"/>
+      <c r="AQ3" s="3"/>
+      <c r="AR3" s="2"/>
+    </row>
+    <row r="4" spans="1:44" s="1" customFormat="1">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1">
+        <v>12342</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2769</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1970</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L1" r:id="rId1"/>
     <hyperlink ref="L2" r:id="rId2"/>
+    <hyperlink ref="L3" r:id="rId3"/>
+    <hyperlink ref="L4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>